<commit_message>
Test Case 1 & Demo file complete
Full mapping using excel read keystrokes for 1 test case complete. Included another python file to test the database values as a check.
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04_MLC\Keystroke_Macros_Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73EEBCB-742C-4506-BE91-12AAE30EA38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAFEDE3-2F78-459E-9E20-11A37EAB5D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="37695" windowHeight="21840" xr2:uid="{66BE3ABC-A902-4477-A0A6-3E79156F8956}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="37695" windowHeight="21840" activeTab="1" xr2:uid="{66BE3ABC-A902-4477-A0A6-3E79156F8956}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Keystrokes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="94">
   <si>
     <t>ASIC Report</t>
   </si>
@@ -40,9 +41,6 @@
     <t>Event 1001: Test legal checklist</t>
   </si>
   <si>
-    <t>1. Is this the first notification</t>
-  </si>
-  <si>
     <t>Update</t>
   </si>
   <si>
@@ -62,6 +60,263 @@
   </si>
   <si>
     <t>10141H CA. 12 DA ASIC Act</t>
+  </si>
+  <si>
+    <t>description of report</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Keystrokes</t>
+  </si>
+  <si>
+    <t>Submit AFS Licensee Details</t>
+  </si>
+  <si>
+    <t>Mapping</t>
+  </si>
+  <si>
+    <t>Keystroke</t>
+  </si>
+  <si>
+    <t>mapping</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Space </t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Input/End section</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Up arrow</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Down arrow </t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Proposed Response</t>
+  </si>
+  <si>
+    <t>[Autofill]</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Depending on where we set the initial click, the number of inputs will change. We can set it to be the centre of the screen for consistency sake</t>
+  </si>
+  <si>
+    <t>--------.</t>
+  </si>
+  <si>
+    <t>Type of Report</t>
+  </si>
+  <si>
+    <t>---.</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Current Details</t>
+  </si>
+  <si>
+    <t>Select on of the following actions. I want to</t>
+  </si>
+  <si>
+    <t>Lodge a report on a significant breach</t>
+  </si>
+  <si>
+    <t>Does the breach also require you to report under s601fc</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>-d</t>
+  </si>
+  <si>
+    <t>Does this report relate to more than one licensee?</t>
+  </si>
+  <si>
+    <t>-d.</t>
+  </si>
+  <si>
+    <t>-d.---.</t>
+  </si>
+  <si>
+    <t>Details of the breach</t>
+  </si>
+  <si>
+    <t>Has Occurred</t>
+  </si>
+  <si>
+    <t>--.</t>
+  </si>
+  <si>
+    <t>Specify Date</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>-x</t>
+  </si>
+  <si>
+    <t>Is breach continuing</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>When was the breach identified</t>
+  </si>
+  <si>
+    <t>When did you become aware that the breach was significant</t>
+  </si>
+  <si>
+    <t>What triggered the investigation of the breach</t>
+  </si>
+  <si>
+    <t>External - Client Compliant(s)</t>
+  </si>
+  <si>
+    <t>-dddddd</t>
+  </si>
+  <si>
+    <t>How many client compliants, that you are aware of, has the licensee received</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>When did you start investigating the nature and scale of the breach (or likely breach)?</t>
+  </si>
+  <si>
+    <t>Have you completed your investigation of the breach (or likely breach)?</t>
+  </si>
+  <si>
+    <t>Provide a date or estimated date for when you will likely complete your investigation</t>
+  </si>
+  <si>
+    <t>--d</t>
+  </si>
+  <si>
+    <t>Nature of the Breach</t>
+  </si>
+  <si>
+    <t>Specify the financial service or product line the breach affected</t>
+  </si>
+  <si>
+    <t>Life Insurance</t>
+  </si>
+  <si>
+    <t>-x---.</t>
+  </si>
+  <si>
+    <t>----dddd</t>
+  </si>
+  <si>
+    <t>Specify the Life insurance Category the breach (or likely breach) affected</t>
+  </si>
+  <si>
+    <t>Non-income stream risk</t>
+  </si>
+  <si>
+    <t>Specify the product the breach (or likely breach) affected</t>
+  </si>
+  <si>
+    <t>Term Life</t>
+  </si>
+  <si>
+    <t>Specify the general category to which the breach (or likely breach) relates</t>
+  </si>
+  <si>
+    <t>-dddd----</t>
+  </si>
+  <si>
+    <t>Specify the issue to which the breach (or likely breach) relates</t>
+  </si>
+  <si>
+    <t>Charges</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>Premiums</t>
+  </si>
+  <si>
+    <t>-ddddd</t>
+  </si>
+  <si>
+    <t>Describe the breach</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>--x</t>
+  </si>
+  <si>
+    <t>Select the name of the Act and relevant section(s) breached (or likely breached)</t>
+  </si>
+  <si>
+    <t>---dd</t>
+  </si>
+  <si>
+    <t>Section/s under the Act</t>
+  </si>
+  <si>
+    <t>Sections</t>
+  </si>
+  <si>
+    <t>Have you reported the circumstances of the breach (or likely breach) to any other regulatory authority?</t>
+  </si>
+  <si>
+    <t>Does the breach (or likely breach) relate to the conduct of your financial advisers or authorised representatives?</t>
+  </si>
+  <si>
+    <t>What are the root causes of the breach (or likely breach)?
+ Cause of breach
+Root cause</t>
+  </si>
+  <si>
+    <t>ASIC Act 2001</t>
+  </si>
+  <si>
+    <t>System Deficiency</t>
+  </si>
+  <si>
+    <t>Specify whether this root cause has been the subject of any internal compliance review or monitoring in the last 3 years</t>
+  </si>
+  <si>
+    <t>Specify the date of any written report or findings (i.e Audit report)</t>
+  </si>
+  <si>
+    <t>---x-----.</t>
+  </si>
+  <si>
+    <t>Extent of the  breach</t>
   </si>
 </sst>
 </file>
@@ -105,10 +360,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83F9240-FB2A-4161-9B85-3E9DE05889B8}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,23 +704,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -469,7 +728,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>44428</v>
@@ -477,13 +736,410 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7CB316F-16CF-4495-8F6D-662F51243827}">
+  <dimension ref="A1:J29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>